<commit_message>
compressible lecture summaries, minor project typos and edits
</commit_message>
<xml_diff>
--- a/projects/Project-2-Data.xlsx
+++ b/projects/Project-2-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3757EC8B-9978-4AA1-8F5C-51003AA8E792}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803AD8A1-6712-46DC-AF71-9140C16FDC2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14680" windowHeight="5870" firstSheet="1" activeTab="1" xr2:uid="{940E1D25-AB1F-4739-9CAC-EFB0F85BAF8F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14680" windowHeight="5870" activeTab="1" xr2:uid="{940E1D25-AB1F-4739-9CAC-EFB0F85BAF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Experiments" sheetId="2" r:id="rId1"/>
@@ -4386,7 +4386,7 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>Caleb has again requested that Power Train "use its god damn knocker" when deciding what to remove and justify it. Just humor him, he's a bit or a nut.</a:t>
+            <a:t>Caleb has again requested that Power Train "use its god damn knocker" when deciding what to remove and justify it. Just humor him, he's a bit of a nut.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6062,8 +6062,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>299831</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6079,7 +6079,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3965381" y="1113835"/>
-          <a:ext cx="4043350" cy="4740865"/>
+          <a:ext cx="4043350" cy="5566365"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6173,6 +6173,21 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
+            <a:t>We have a significant variance in the measurments, but that can be quantified and considered when optimizing. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
             <a:t>Combustion Team,</a:t>
           </a:r>
         </a:p>
@@ -6227,15 +6242,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1501581</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>174035</xdr:rowOff>
+      <xdr:colOff>1463481</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>148635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>299831</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:colOff>261731</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6250,7 +6265,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3965381" y="6193835"/>
+          <a:off x="3927281" y="9406935"/>
           <a:ext cx="4043350" cy="4156665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6330,7 +6345,7 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>10-20 min shoudl do.</a:t>
+            <a:t>10-20 min should do.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6714,7 +6729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBFA7722-0990-425A-9082-C1730BC08B08}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
@@ -9012,8 +9027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7185D0CF-D6CC-453E-94B4-FEEA5C86784B}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S61" sqref="S61"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="T66" sqref="T66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10636,7 +10651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1B521F-BAF1-4BD8-A8C0-680B76C08FBF}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
@@ -10944,7 +10959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87006A56-0547-4E31-BBEF-15C020FA07F0}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
lecture 18 notes uploaded, oblique shocks
</commit_message>
<xml_diff>
--- a/projects/Project-2-Data.xlsx
+++ b/projects/Project-2-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20358"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20359"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smohler\ME322-S20\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803AD8A1-6712-46DC-AF71-9140C16FDC2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8328CD78-B52D-4B02-B50B-4BF4A4DF7A2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14680" windowHeight="5870" activeTab="1" xr2:uid="{940E1D25-AB1F-4739-9CAC-EFB0F85BAF8F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14680" windowHeight="5870" firstSheet="1" activeTab="3" xr2:uid="{940E1D25-AB1F-4739-9CAC-EFB0F85BAF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Experiments" sheetId="2" r:id="rId1"/>
@@ -1515,13 +1515,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1531,15 +1540,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1581,6 +1581,1113 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Combustion Efficiency'!$A$3:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Combustion Efficiency'!$B$3:$B$46</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>0.48109676462297751</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.48434519408810428</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44375378958452633</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48504488505932375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44643731394881425</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40642998921708806</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45828233332249813</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43710555693670256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.48398515763906108</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25559784295163085</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.50467519515020931</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.31336419473150023</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.50483276758221451</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.42941056955978851</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.31064948870233311</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.46420709368432522</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.49059519621531261</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.27918439249395666</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.4593321114740111</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.48503299168295433</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.40444405581978027</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47401504276354356</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.41107362599136987</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.4752847226391409</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.48661436978583739</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.23008676589103702</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.46684966355012841</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.46056282001855153</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.4039929242749235</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.48206050107863196</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.34351964460430906</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.39277525079738157</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.23944388539739E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.42975715665959235</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.54064465703253894</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.3303635489035681E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.40303219247109445</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.40880164812985237</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.4396940226621126</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.38156870729956893</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.44156968619041875</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.48430177231297661</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43707408037052481</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8859-4309-AFEC-01CF57553E97}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1995037679"/>
+        <c:axId val="2080561807"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1995037679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2080561807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2080561807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1995037679"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6427,6 +7534,42 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>975178</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>128814</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62CF7202-93DF-4667-A34B-6363572F2FD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6754,14 +7897,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20" thickBot="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="66"/>
+      <c r="D1" s="68"/>
       <c r="E1" s="9">
         <f>COUNT(A3:A33)</f>
         <v>31</v>
@@ -6797,16 +7940,16 @@
       <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="71" t="s">
+      <c r="M2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71" t="s">
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="71"/>
+      <c r="R2" s="74"/>
     </row>
     <row r="3" spans="1:18" ht="15.5" thickTop="1">
       <c r="A3" s="37">
@@ -6822,13 +7965,13 @@
       <c r="E3" s="34">
         <v>28.964749277906975</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="L3" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="69" t="s">
+      <c r="M3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="69" t="s">
+      <c r="N3" s="72" t="s">
         <v>4</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -6837,7 +7980,7 @@
       <c r="P3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="69" t="s">
+      <c r="Q3" s="72" t="s">
         <v>9</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -6858,16 +8001,16 @@
       <c r="E4" s="34">
         <v>0.46871711653315556</v>
       </c>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="70"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
       <c r="O4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="70"/>
+      <c r="Q4" s="73"/>
       <c r="R4" s="3" t="s">
         <v>11</v>
       </c>
@@ -7204,13 +8347,13 @@
       <c r="E15" s="34">
         <v>4.9092516445540966</v>
       </c>
-      <c r="L15" s="72" t="s">
+      <c r="L15" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="73"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="73"/>
-      <c r="P15" s="74"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="70"/>
+      <c r="O15" s="70"/>
+      <c r="P15" s="71"/>
     </row>
     <row r="16" spans="1:18" ht="15.5" thickBot="1">
       <c r="A16" s="37">
@@ -7709,14 +8852,14 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="19">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="66" t="s">
+      <c r="B34" s="67"/>
+      <c r="C34" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="66"/>
+      <c r="D34" s="68"/>
       <c r="E34" s="9">
         <f>COUNT(A36:A69)</f>
         <v>34</v>
@@ -8265,14 +9408,14 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="19">
-      <c r="A71" s="67" t="s">
+      <c r="A71" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="68"/>
-      <c r="C71" s="66" t="s">
+      <c r="B71" s="67"/>
+      <c r="C71" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="66"/>
+      <c r="D71" s="68"/>
       <c r="E71" s="9">
         <f>COUNT(A73:A116)</f>
         <v>44</v>
@@ -9003,11 +10146,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="L15:P15"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="Q3:Q4"/>
@@ -9016,6 +10154,11 @@
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="L15:P15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9027,7 +10170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7185D0CF-D6CC-453E-94B4-FEEA5C86784B}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="T66" sqref="T66"/>
     </sheetView>
   </sheetViews>
@@ -10959,8 +12102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87006A56-0547-4E31-BBEF-15C020FA07F0}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>